<commit_message>
new scripts that try to integrate the plot builder inside the report builder, still work in process, we are modigying an excel file too to carry tests
</commit_message>
<xml_diff>
--- a/excel_books/art8_spashares10_data_prototype.xlsx
+++ b/excel_books/art8_spashares10_data_prototype.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n740789\Documents\sfdr_report_generator\excel_books\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CEA62BB-9EB7-4693-ACB8-48D0D9156EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90398EF-F9D9-4E64-85F7-C96C75AD5712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10960" xr2:uid="{1B159470-F773-48C5-9E2D-13C769AF5DFC}"/>
+    <workbookView xWindow="-3075" yWindow="-21720" windowWidth="38640" windowHeight="21840" xr2:uid="{1B159470-F773-48C5-9E2D-13C769AF5DFC}"/>
   </bookViews>
   <sheets>
     <sheet name="art8_spshare10_holders" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="75">
   <si>
     <t>{{PRODUCT_NAME}}</t>
   </si>
@@ -255,6 +255,12 @@
   </si>
   <si>
     <t>total_opex_rest_sbexcluded</t>
+  </si>
+  <si>
+    <t>FIG05241</t>
+  </si>
+  <si>
+    <t>FIG05242</t>
   </si>
 </sst>
 </file>
@@ -264,7 +270,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,6 +294,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -350,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -362,6 +374,7 @@
     <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,32 +709,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF59C17-7886-4FAC-8A2A-DD65BB55176D}">
-  <dimension ref="A1:AP4"/>
+  <dimension ref="A1:AS4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AL19" sqref="AL19"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="116" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="42.1796875" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6328125" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="31.54296875" hidden="1" customWidth="1"/>
-    <col min="4" max="5" width="37" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="35.36328125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="31" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="32" hidden="1" customWidth="1"/>
-    <col min="9" max="10" width="25.81640625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="29.36328125" hidden="1" customWidth="1"/>
-    <col min="12" max="22" width="40.26953125" customWidth="1"/>
-    <col min="23" max="29" width="31.1796875" customWidth="1"/>
-    <col min="30" max="30" width="37.26953125" customWidth="1"/>
-    <col min="31" max="39" width="31.1796875" customWidth="1"/>
-    <col min="40" max="40" width="35.54296875" customWidth="1"/>
-    <col min="41" max="42" width="31.1796875" customWidth="1"/>
+    <col min="1" max="1" width="42.1796875" customWidth="1"/>
+    <col min="2" max="2" width="14.6328125" customWidth="1"/>
+    <col min="3" max="3" width="31.54296875" customWidth="1"/>
+    <col min="4" max="5" width="37" customWidth="1"/>
+    <col min="6" max="6" width="35.36328125" customWidth="1"/>
+    <col min="7" max="7" width="31" customWidth="1"/>
+    <col min="8" max="8" width="32" customWidth="1"/>
+    <col min="9" max="10" width="25.81640625" customWidth="1"/>
+    <col min="11" max="11" width="29.36328125" customWidth="1"/>
+    <col min="12" max="14" width="40.26953125" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="20" customWidth="1"/>
+    <col min="16" max="16" width="20" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="20" customWidth="1"/>
+    <col min="18" max="18" width="20" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="20" customWidth="1"/>
+    <col min="20" max="20" width="20" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="20" customWidth="1"/>
+    <col min="22" max="22" width="20" hidden="1" customWidth="1"/>
+    <col min="23" max="25" width="20" customWidth="1"/>
+    <col min="26" max="26" width="20" hidden="1" customWidth="1"/>
+    <col min="27" max="29" width="20" customWidth="1"/>
+    <col min="30" max="30" width="20" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="20" customWidth="1"/>
+    <col min="32" max="32" width="31" hidden="1" customWidth="1"/>
+    <col min="33" max="39" width="31.1796875" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="35.54296875" hidden="1" customWidth="1"/>
+    <col min="41" max="42" width="31.1796875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:45" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -849,7 +874,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -976,8 +1001,16 @@
       <c r="AP2" s="4">
         <v>87.104060710767754</v>
       </c>
+      <c r="AR2" s="5">
+        <f>SUM(O2,Q2,S2,U2)</f>
+        <v>100</v>
+      </c>
+      <c r="AS2" s="5">
+        <f>SUM(P2,R2,T2,V2)</f>
+        <v>100</v>
+      </c>
     </row>
-    <row r="3" spans="1:42" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:45" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1011,8 +1044,109 @@
       <c r="K3" t="s">
         <v>25</v>
       </c>
+      <c r="L3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="M3" s="4">
+        <v>15</v>
+      </c>
+      <c r="N3" s="4">
+        <v>7.8</v>
+      </c>
+      <c r="O3" s="4">
+        <v>10</v>
+      </c>
+      <c r="P3" s="4">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>15</v>
+      </c>
+      <c r="R3" s="4">
+        <v>1.2058226002383259E-2</v>
+      </c>
+      <c r="S3" s="4">
+        <v>23</v>
+      </c>
+      <c r="T3" s="4">
+        <v>12.933952195196932</v>
+      </c>
+      <c r="U3" s="4">
+        <v>52</v>
+      </c>
+      <c r="V3" s="4">
+        <v>87.052608574870163</v>
+      </c>
+      <c r="W3" s="4">
+        <v>8.3335808462373091</v>
+      </c>
+      <c r="X3" s="4">
+        <v>17.287010163102899</v>
+      </c>
+      <c r="Y3" s="4">
+        <v>5.7018250682419917E-3</v>
+      </c>
+      <c r="Z3" s="4">
+        <v>3.1055411770953734E-3</v>
+      </c>
+      <c r="AA3" s="4">
+        <v>2.272836178794166E-3</v>
+      </c>
+      <c r="AB3" s="4">
+        <v>4.9221907035977104E-3</v>
+      </c>
+      <c r="AC3" s="4">
+        <v>8.3256061849902725</v>
+      </c>
+      <c r="AD3" s="4">
+        <v>17.278982431222204</v>
+      </c>
+      <c r="AE3" s="4">
+        <v>91.666419153762689</v>
+      </c>
+      <c r="AF3" s="4">
+        <v>82.712989836897094</v>
+      </c>
+      <c r="AG3" s="4">
+        <v>6.2726957508903416</v>
+      </c>
+      <c r="AH3" s="4">
+        <v>12.895939289232246</v>
+      </c>
+      <c r="AI3" s="4">
+        <v>2.0304323731814067E-4</v>
+      </c>
+      <c r="AJ3" s="4">
+        <v>4.3972264454447772E-4</v>
+      </c>
+      <c r="AK3" s="4">
+        <v>3.496150742571735E-3</v>
+      </c>
+      <c r="AL3" s="4">
+        <v>7.5714742857502255E-3</v>
+      </c>
+      <c r="AM3" s="4">
+        <v>6.2689965569104515</v>
+      </c>
+      <c r="AN3" s="4">
+        <v>12.887928092301951</v>
+      </c>
+      <c r="AO3" s="4">
+        <v>93.727304249109665</v>
+      </c>
+      <c r="AP3" s="4">
+        <v>87.104060710767754</v>
+      </c>
+      <c r="AR3" s="5">
+        <f>SUM(O3,Q3,S3,U3)</f>
+        <v>100</v>
+      </c>
+      <c r="AS3" s="5">
+        <f>SUM(P3,R3,T3,V3)</f>
+        <v>109.99861899606948</v>
+      </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1046,8 +1180,110 @@
       <c r="K4" t="s">
         <v>37</v>
       </c>
+      <c r="L4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="M4" s="4">
+        <v>12.947391425129837</v>
+      </c>
+      <c r="N4" s="4">
+        <v>6.2392023967425745</v>
+      </c>
+      <c r="O4" s="4">
+        <v>15</v>
+      </c>
+      <c r="P4" s="4">
+        <v>1.3810039305225002E-3</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>20</v>
+      </c>
+      <c r="R4" s="4">
+        <v>1.2058226002383259E-2</v>
+      </c>
+      <c r="S4" s="4">
+        <v>35</v>
+      </c>
+      <c r="T4" s="4">
+        <v>12.933952195196932</v>
+      </c>
+      <c r="U4" s="4">
+        <v>30</v>
+      </c>
+      <c r="V4" s="4">
+        <v>87.052608574870163</v>
+      </c>
+      <c r="W4" s="4">
+        <v>8.3335808462373091</v>
+      </c>
+      <c r="X4" s="4">
+        <v>17.287010163102899</v>
+      </c>
+      <c r="Y4" s="4">
+        <v>5.7018250682419917E-3</v>
+      </c>
+      <c r="Z4" s="4">
+        <v>3.1055411770953734E-3</v>
+      </c>
+      <c r="AA4" s="4">
+        <v>2.272836178794166E-3</v>
+      </c>
+      <c r="AB4" s="4">
+        <v>4.9221907035977104E-3</v>
+      </c>
+      <c r="AC4" s="4">
+        <v>8.3256061849902725</v>
+      </c>
+      <c r="AD4" s="4">
+        <v>17.278982431222204</v>
+      </c>
+      <c r="AE4" s="4">
+        <v>91.666419153762689</v>
+      </c>
+      <c r="AF4" s="4">
+        <v>82.712989836897094</v>
+      </c>
+      <c r="AG4" s="4">
+        <v>6.2726957508903416</v>
+      </c>
+      <c r="AH4" s="4">
+        <v>12.895939289232246</v>
+      </c>
+      <c r="AI4" s="4">
+        <v>2.0304323731814067E-4</v>
+      </c>
+      <c r="AJ4" s="4">
+        <v>4.3972264454447772E-4</v>
+      </c>
+      <c r="AK4" s="4">
+        <v>3.496150742571735E-3</v>
+      </c>
+      <c r="AL4" s="4">
+        <v>7.5714742857502255E-3</v>
+      </c>
+      <c r="AM4" s="4">
+        <v>6.2689965569104515</v>
+      </c>
+      <c r="AN4" s="4">
+        <v>12.887928092301951</v>
+      </c>
+      <c r="AO4" s="4">
+        <v>93.727304249109665</v>
+      </c>
+      <c r="AP4" s="4">
+        <v>87.104060710767754</v>
+      </c>
+      <c r="AR4" s="5">
+        <f t="shared" ref="AR3:AR4" si="0">SUM(O4,Q4,S4,U4)</f>
+        <v>100</v>
+      </c>
+      <c r="AS4" s="5">
+        <f t="shared" ref="AS3:AS4" si="1">SUM(P4,R4,T4,V4)</f>
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>